<commit_message>
code cleaning and adding comments
</commit_message>
<xml_diff>
--- a/content/exemplo.xlsx
+++ b/content/exemplo.xlsx
@@ -10,14 +10,13 @@
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
-    <sheet name="Now" r:id="rId7" sheetId="4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>id</t>
   </si>
@@ -59,58 +58,12 @@
   </si>
   <si>
     <t>7885522117799</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Code Type</t>
-  </si>
-  <si>
-    <t>Brand Suggested</t>
-  </si>
-  <si>
-    <t>7891150000018</t>
-  </si>
-  <si>
-    <t>GTIN-13</t>
-  </si>
-  <si>
-    <t>7891150016736</t>
-  </si>
-  <si>
-    <t>7896055501103</t>
-  </si>
-  <si>
-    <t>7891150032729</t>
-  </si>
-  <si>
-    <t>7896007540631</t>
-  </si>
-  <si>
-    <t>7896902209114</t>
-  </si>
-  <si>
-    <t>7891010560737</t>
-  </si>
-  <si>
-    <t>7891010032937</t>
-  </si>
-  <si>
-    <t>7898095296018</t>
-  </si>
-  <si>
-    <t>7898422746759</t>
-  </si>
-  <si>
-    <t>Código Interno</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -447,16 +400,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="86.140625" collapsed="false"/>
+    <col min="2" max="2" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="86.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -519,10 +472,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>7896007540631</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
+        <v>665544</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -530,10 +480,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>7896902209114</v>
+        <v>7896007540631</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -541,10 +491,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>7891010560737</v>
+        <v>7896902209114</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -552,10 +502,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>7891010032937</v>
+        <v>7891010560737</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -563,10 +513,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>7898095296018</v>
+        <v>7891010032937</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -574,17 +524,28 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>7898422746759</v>
+        <v>7898095296018</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="1">
+        <v>7898422746759</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -616,127 +577,4 @@
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12"/>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
 </file>
</xml_diff>